<commit_message>
WIP Updating objects and scripts for new interactions
Fixed all drawers and grabbable objects in main scene to use Grab Interactables; removed obsolete scripts, added Locked and Used classes, started redoing the checks that happen on interactions that will need scripting, but did not finish
</commit_message>
<xml_diff>
--- a/NewRecipeInteractionChange.xlsx
+++ b/NewRecipeInteractionChange.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnityProjects\TheNewRecipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29869B2C-289C-4821-9AC8-9102BA88EFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D77CE73-5178-44ED-BBEA-B61876487B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{1E202066-871A-4457-8B13-6F9D6941ED9F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1E202066-871A-4457-8B13-6F9D6941ED9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="116">
   <si>
     <t>Script</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Used to reparent objects that are in the drawer</t>
   </si>
   <si>
-    <t>May not need to change, except possibly to change OnCollisionEnter to OnTriggerEnter (player is now trigger)</t>
-  </si>
-  <si>
     <t>DumbwaiterDoor</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>Superclass of Grabbables!!</t>
   </si>
   <si>
-    <t xml:space="preserve">Properties of "Used" and "Locked"; add Rigidbodies and toggle physics; </t>
-  </si>
-  <si>
     <t>Grab with Joint</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
     <t>Returns drawers with animation</t>
   </si>
   <si>
-    <t>See what socket looks like - may add animation to Select Exit event instead (when drawer is dropped)</t>
-  </si>
-  <si>
     <t>Paragraph</t>
   </si>
   <si>
@@ -330,9 +321,6 @@
     <t>Wine bottles</t>
   </si>
   <si>
-    <t>Taps</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -352,6 +340,51 @@
   </si>
   <si>
     <t>Add attach tranforms</t>
+  </si>
+  <si>
+    <t>Notes of what I did:</t>
+  </si>
+  <si>
+    <t>Removed Throwable Object, added Grab Interactable (Throw on detach)</t>
+  </si>
+  <si>
+    <t>Removed Grabbable Object, added Grab Interactable (Kinematic)</t>
+  </si>
+  <si>
+    <t>Removed Grabbable Object, added Grab Interactable (Not using Gravity)</t>
+  </si>
+  <si>
+    <t>Removed Grabbable Object, added Grab Interactable</t>
+  </si>
+  <si>
+    <t>Taps (Drawer)</t>
+  </si>
+  <si>
+    <t>Taps (World)</t>
+  </si>
+  <si>
+    <t>Do not add gravity on detach if they go to inventory</t>
+  </si>
+  <si>
+    <t>Removed Grabbable Object, added Grab Interactable (Use Gravity)</t>
+  </si>
+  <si>
+    <t>Weren't grabbable - fix this in next sprint</t>
+  </si>
+  <si>
+    <t>May not need at all - try without (deleted)</t>
+  </si>
+  <si>
+    <t>Deleted</t>
+  </si>
+  <si>
+    <t>Properties of "Used" and "Locked"; add Rigidbodies and toggle physics; wrote new "UsableObject" and "LockableObject"</t>
+  </si>
+  <si>
+    <t>Works without this (backstopped by collider) - deleted</t>
+  </si>
+  <si>
+    <t>Not used in scene - deleted</t>
   </si>
 </sst>
 </file>
@@ -375,7 +408,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,6 +418,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,10 +440,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,16 +761,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30CEBF79-7071-4366-8D05-0ACFB656B3B9}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="57.5703125" customWidth="1"/>
-    <col min="4" max="4" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.42578125" customWidth="1"/>
+    <col min="4" max="4" width="100.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -760,7 +800,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,250 +811,256 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
+      <c r="A4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>35</v>
+      <c r="A7" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>36</v>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
         <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" t="s">
         <v>73</v>
-      </c>
-      <c r="B16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1022,23 +1068,23 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,79 +1092,79 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
         <v>12</v>
-      </c>
-      <c r="B29" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
         <v>24</v>
-      </c>
-      <c r="B31" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1129,76 +1175,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0AB0D18-DA47-4884-BF9D-FDCB350AE906}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>95</v>
       </c>
-      <c r="C2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>96</v>
       </c>
-      <c r="C3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>104</v>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP Revised gameplay scripts
Made changes to gameplay scripts that were incorporated into interactions, testing gameplay
</commit_message>
<xml_diff>
--- a/NewRecipeInteractionChange.xlsx
+++ b/NewRecipeInteractionChange.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnityProjects\TheNewRecipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D77CE73-5178-44ED-BBEA-B61876487B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA654E8B-23C8-474F-846E-7D799B2289BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1E202066-871A-4457-8B13-6F9D6941ED9F}"/>
+    <workbookView xWindow="2430" yWindow="1200" windowWidth="21600" windowHeight="12450" xr2:uid="{1E202066-871A-4457-8B13-6F9D6941ED9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts" sheetId="1" r:id="rId1"/>
@@ -216,9 +216,6 @@
     <t>Inherits from GrabbableObject: Not used? May be inherited</t>
   </si>
   <si>
-    <t>Adds and removes joints and controls velocities - may not be required</t>
-  </si>
-  <si>
     <t>PushableObject</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>TapSensor</t>
   </si>
   <si>
-    <t>Uses "Used" property of Grabbable Object</t>
-  </si>
-  <si>
     <t>Grab Interactable/Socket</t>
   </si>
   <si>
@@ -258,9 +252,6 @@
     <t>Teleportation</t>
   </si>
   <si>
-    <t>None: can be entirely replaced with toolkit</t>
-  </si>
-  <si>
     <t>ThrowableObject</t>
   </si>
   <si>
@@ -270,27 +261,18 @@
     <t>Inherits from GrabbableObject: Inherited by ThrowableObject</t>
   </si>
   <si>
-    <t>Nothing game related - just replace</t>
-  </si>
-  <si>
     <t>TouchableObject</t>
   </si>
   <si>
     <t>Not used in scene</t>
   </si>
   <si>
-    <t>If used, would be replacable with Grab Interactable Hover</t>
-  </si>
-  <si>
     <t>Turning</t>
   </si>
   <si>
     <t>Turns player</t>
   </si>
   <si>
-    <t>Completely replaceable with Snap Turn</t>
-  </si>
-  <si>
     <t>WineSlot</t>
   </si>
   <si>
@@ -385,6 +367,24 @@
   </si>
   <si>
     <t>Not used in scene - deleted</t>
+  </si>
+  <si>
+    <t>None: can be entirely replaced with toolkit (deleted)</t>
+  </si>
+  <si>
+    <t>Completely replaceable with Snap Turn (deleted)</t>
+  </si>
+  <si>
+    <t>If used, would be replacable with Grab Interactable Hover (deleted</t>
+  </si>
+  <si>
+    <t>Nothing game related - just replace (deleted)</t>
+  </si>
+  <si>
+    <t>Uses "Used" property of Grabbable Object (NR)</t>
+  </si>
+  <si>
+    <t>Adds and removes joints and controls velocities - may not be required (deleted)</t>
   </si>
 </sst>
 </file>
@@ -762,14 +762,14 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="56.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" customWidth="1"/>
     <col min="4" max="4" width="100.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.85546875" bestFit="1" customWidth="1"/>
@@ -800,7 +800,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -814,7 +814,7 @@
         <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -828,7 +828,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,10 +839,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -926,7 +926,7 @@
         <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -968,91 +968,91 @@
         <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
         <v>66</v>
       </c>
-      <c r="B15" t="s">
-        <v>68</v>
-      </c>
       <c r="C15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" t="s">
         <v>67</v>
-      </c>
-      <c r="D15" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" t="s">
-        <v>72</v>
-      </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,34 +1137,34 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s">
         <v>60</v>
-      </c>
-      <c r="B34" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
         <v>62</v>
-      </c>
-      <c r="B35" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
         <v>64</v>
-      </c>
-      <c r="B36" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1191,95 +1191,95 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
         <v>93</v>
-      </c>
-      <c r="D3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
         <v>96</v>
-      </c>
-      <c r="B8" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>